<commit_message>
updated WoRMS processed data
</commit_message>
<xml_diff>
--- a/processed_data/WoRMS_taxlist_20250211_processed.xlsx
+++ b/processed_data/WoRMS_taxlist_20250211_processed.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanasevigny/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanasevigny/git/ENSO_CalCOFI_dispersals2024/processed_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8484EDF3-A607-6A47-BC71-5AF06440B479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F6817F-4BB6-E641-96C7-469C2535D189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-220" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="WoRMS download 2025-02-11" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'WoRMS download 2025-02-11'!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'WoRMS download 2025-02-11'!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="270">
   <si>
     <t>AphiaID</t>
   </si>
@@ -784,9 +784,6 @@
     <t>JKS Notes for Exclusion</t>
   </si>
   <si>
-    <t>JKS Notes for maybe exclusion</t>
-  </si>
-  <si>
     <t>microscopic worms</t>
   </si>
   <si>
@@ -827,9 +824,6 @@
   </si>
   <si>
     <t>outdated name (replaced with other in the list)</t>
-  </si>
-  <si>
-    <t>acorn worm</t>
   </si>
   <si>
     <t>small worms</t>
@@ -1190,10 +1184,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H234"/>
+  <dimension ref="A1:G234"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H113" sqref="H113"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1204,7 +1198,7 @@
     <col min="7" max="7" width="31.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1226,11 +1220,8 @@
       <c r="G1" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>20300</v>
       </c>
@@ -1253,7 +1244,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>20285</v>
       </c>
@@ -1276,7 +1267,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>14165</v>
       </c>
@@ -1296,7 +1287,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1019642</v>
       </c>
@@ -1316,10 +1307,10 @@
         <v>4</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>883</v>
       </c>
@@ -1339,7 +1330,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1300</v>
       </c>
@@ -1362,7 +1353,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1069</v>
       </c>
@@ -1382,11 +1373,10 @@
         <v>4</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>150314</v>
       </c>
@@ -1406,11 +1396,10 @@
         <v>4</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>1304</v>
       </c>
@@ -1433,7 +1422,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>1080</v>
       </c>
@@ -1453,11 +1442,10 @@
         <v>4</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>889925</v>
       </c>
@@ -1477,11 +1465,10 @@
         <v>4</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>1278</v>
       </c>
@@ -1504,7 +1491,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>845958</v>
       </c>
@@ -1524,10 +1511,10 @@
         <v>4</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>1071</v>
       </c>
@@ -1547,7 +1534,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>1070</v>
       </c>
@@ -1567,7 +1554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>150507</v>
       </c>
@@ -1587,7 +1574,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>1078</v>
       </c>
@@ -1607,10 +1594,10 @@
         <v>4</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>384687</v>
       </c>
@@ -1632,9 +1619,8 @@
       <c r="G19" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>1302</v>
       </c>
@@ -1654,7 +1640,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>1067</v>
       </c>
@@ -1674,10 +1660,10 @@
         <v>4</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>394515</v>
       </c>
@@ -1700,7 +1686,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>1083</v>
       </c>
@@ -1720,10 +1706,10 @@
         <v>4</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>22388</v>
       </c>
@@ -1743,7 +1729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>147803</v>
       </c>
@@ -1763,7 +1749,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>104019</v>
       </c>
@@ -1783,7 +1769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>235154</v>
       </c>
@@ -1803,7 +1789,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>104020</v>
       </c>
@@ -1823,7 +1809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>1795</v>
       </c>
@@ -1843,7 +1829,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>1794</v>
       </c>
@@ -1863,7 +1849,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>5949</v>
       </c>
@@ -1883,10 +1869,10 @@
         <v>4</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>146421</v>
       </c>
@@ -2357,7 +2343,7 @@
         <v>4</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.15">
@@ -2586,7 +2572,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A65">
         <v>1596250</v>
       </c>
@@ -2606,7 +2592,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A66">
         <v>123080</v>
       </c>
@@ -2626,7 +2612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A67">
         <v>1601453</v>
       </c>
@@ -2646,7 +2632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A68">
         <v>123081</v>
       </c>
@@ -2666,7 +2652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A69">
         <v>1601455</v>
       </c>
@@ -2686,7 +2672,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A70">
         <v>123082</v>
       </c>
@@ -2706,7 +2692,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A71">
         <v>1601456</v>
       </c>
@@ -2726,7 +2712,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A72">
         <v>149846</v>
       </c>
@@ -2746,7 +2732,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A73">
         <v>123083</v>
       </c>
@@ -2766,7 +2752,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A74">
         <v>1601457</v>
       </c>
@@ -2786,7 +2772,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A75">
         <v>1596244</v>
       </c>
@@ -2806,10 +2792,10 @@
         <v>4</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.15">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A76">
         <v>123084</v>
       </c>
@@ -2829,7 +2815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A77">
         <v>1601454</v>
       </c>
@@ -2849,7 +2835,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A78">
         <v>148745</v>
       </c>
@@ -2869,7 +2855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A79">
         <v>1820</v>
       </c>
@@ -2888,11 +2874,8 @@
       <c r="F79" t="s">
         <v>4</v>
       </c>
-      <c r="H79" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.15">
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A80">
         <v>579849</v>
       </c>
@@ -2952,7 +2935,7 @@
         <v>4</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.15">
@@ -2975,7 +2958,7 @@
         <v>4</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.15">
@@ -2998,7 +2981,7 @@
         <v>4</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.15">
@@ -3061,7 +3044,7 @@
         <v>4</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.15">
@@ -3244,7 +3227,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A97">
         <v>104</v>
       </c>
@@ -3264,7 +3247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A98">
         <v>1582101</v>
       </c>
@@ -3284,7 +3267,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A99">
         <v>2094</v>
       </c>
@@ -3304,7 +3287,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A100">
         <v>2132</v>
       </c>
@@ -3324,10 +3307,10 @@
         <v>4</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.15">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A101">
         <v>731848</v>
       </c>
@@ -3347,10 +3330,10 @@
         <v>4</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.15">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A102">
         <v>834422</v>
       </c>
@@ -3370,10 +3353,10 @@
         <v>4</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.15">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A103">
         <v>22945</v>
       </c>
@@ -3392,11 +3375,11 @@
       <c r="F103" t="s">
         <v>4</v>
       </c>
-      <c r="H103" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="G103" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A104">
         <v>2133</v>
       </c>
@@ -3416,10 +3399,10 @@
         <v>4</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.15">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A105">
         <v>178814</v>
       </c>
@@ -3439,10 +3422,10 @@
         <v>4</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.15">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A106">
         <v>162563</v>
       </c>
@@ -3462,10 +3445,10 @@
         <v>4</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.15">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A107">
         <v>1761571</v>
       </c>
@@ -3485,10 +3468,10 @@
         <v>4</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.15">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A108">
         <v>162760</v>
       </c>
@@ -3508,10 +3491,10 @@
         <v>4</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.15">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A109">
         <v>1293</v>
       </c>
@@ -3531,7 +3514,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A110">
         <v>1502208</v>
       </c>
@@ -3551,7 +3534,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A111">
         <v>1294</v>
       </c>
@@ -3571,7 +3554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A112">
         <v>122309</v>
       </c>
@@ -3591,7 +3574,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A113">
         <v>146899</v>
       </c>
@@ -3610,11 +3593,11 @@
       <c r="F113" t="s">
         <v>4</v>
       </c>
-      <c r="H113" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="G113" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A114">
         <v>122307</v>
       </c>
@@ -3634,7 +3617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A115">
         <v>1320351</v>
       </c>
@@ -3654,7 +3637,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A116">
         <v>1652337</v>
       </c>
@@ -3674,10 +3657,10 @@
         <v>4</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.15">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A117">
         <v>1652332</v>
       </c>
@@ -3697,10 +3680,10 @@
         <v>4</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.15">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A118">
         <v>1051</v>
       </c>
@@ -3720,10 +3703,10 @@
         <v>4</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.15">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A119">
         <v>798</v>
       </c>
@@ -3743,10 +3726,10 @@
         <v>4</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.15">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A120">
         <v>717338</v>
       </c>
@@ -3766,10 +3749,10 @@
         <v>4</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.15">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A121">
         <v>1724992</v>
       </c>
@@ -3789,10 +3772,10 @@
         <v>4</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.15">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A122">
         <v>1724993</v>
       </c>
@@ -3812,10 +3795,10 @@
         <v>4</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.15">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A123">
         <v>19948</v>
       </c>
@@ -3835,10 +3818,10 @@
         <v>4</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.15">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A124">
         <v>794</v>
       </c>
@@ -3858,7 +3841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A125">
         <v>853042</v>
       </c>
@@ -3878,7 +3861,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A126">
         <v>1298</v>
       </c>
@@ -3898,7 +3881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A127">
         <v>559</v>
       </c>
@@ -3918,7 +3901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A128">
         <v>886287</v>
       </c>
@@ -4098,7 +4081,7 @@
         <v>4</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.15">
@@ -4121,7 +4104,7 @@
         <v>4</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.15">
@@ -4144,7 +4127,7 @@
         <v>4</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.15">
@@ -4167,7 +4150,7 @@
         <v>4</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.15">
@@ -4190,7 +4173,7 @@
         <v>4</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.15">
@@ -5792,7 +5775,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>